<commit_message>
changed canonical to example.org/ig/example
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-MyCIBMTRPatient.xlsx
+++ b/docs/StructureDefinition-MyCIBMTRPatient.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://example.org/StructureDefinition/MyCIBMTRPatient</t>
+    <t>http://example.org/ig/example/StructureDefinition/MyCIBMTRPatient</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-20T09:15:43-05:00</t>
+    <t>2023-04-26T11:15:05-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -105,7 +105,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://example.org/StructureDefinition/MyUSCorePatient</t>
+    <t>http://example.org/ig/example/StructureDefinition/MyUSCorePatient</t>
   </si>
   <si>
     <t>Abstract</t>

</xml_diff>

<commit_message>
added publication directory and Dockerfile for creating site on localhost
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-MyCIBMTRPatient.xlsx
+++ b/docs/StructureDefinition-MyCIBMTRPatient.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://example.org/ig/example/StructureDefinition/MyCIBMTRPatient</t>
+    <t>http://example.org/ig/exampleig/StructureDefinition/MyCIBMTRPatient</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-26T11:15:05-05:00</t>
+    <t>2023-04-27T11:07:01-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -105,7 +105,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://example.org/ig/example/StructureDefinition/MyUSCorePatient</t>
+    <t>http://example.org/ig/exampleig/StructureDefinition/MyUSCorePatient</t>
   </si>
   <si>
     <t>Abstract</t>

</xml_diff>